<commit_message>
start develop.py for monthly_report
</commit_message>
<xml_diff>
--- a/blank/work.xlsx
+++ b/blank/work.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Суточный отчет электротехнического персонала по обслуживанию электрооборудования производственной базы, буровой установки и бригадных хозяйств</t>
   </si>
@@ -59,16 +59,10 @@
   </si>
   <si>
     <t xml:space="preserve">напряжение питания кВ :                                                     .             ВН                  НН                           08.00ч.          6.3кВ  51А      0.69кВ  0.526А                                                                                                20.00ч.          6.3кВ  52А      0.4кВ     512А                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Инженер-электроник Черенков А.В. 4 гр. до и выше 1000В. Дата след.проверки 26.11.2022</t>
   </si>
   <si>
     <t xml:space="preserve">2. Работы согласно графика ППР : 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Электромонтер дневн. Гурьянов ВА  Персонал ОГЭ, 4 гр до и выше 1000В. Дата след. проверки 12.11.2022</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -580,8 +574,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -589,7 +583,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.98"/>
@@ -679,22 +673,18 @@
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
-      <c r="F6" s="21" t="s">
-        <v>13</v>
-      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="25" t="s">
-        <v>15</v>
-      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="22"/>
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
@@ -706,7 +696,7 @@
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="22"/>
@@ -762,7 +752,7 @@
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>

</xml_diff>

<commit_message>
work with develop: add monthly report, not finish
</commit_message>
<xml_diff>
--- a/blank/work.xlsx
+++ b/blank/work.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Суточный отчет электротехнического персонала по обслуживанию электрооборудования производственной базы, буровой установки и бригадных хозяйств</t>
   </si>
@@ -59,10 +59,16 @@
   </si>
   <si>
     <t xml:space="preserve">напряжение питания кВ :                                                     .             ВН                  НН                           08.00ч.          6.3кВ  51А      0.69кВ  0.526А                                                                                                20.00ч.          6.3кВ  52А      0.4кВ     512А                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Инженер-электроник, 4гр Черенков А.В. 4гр.</t>
   </si>
   <si>
     <t xml:space="preserve">2. Работы согласно графика ППР : 
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Электромонтер, 4гр Гурьянов В.А.</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -78,7 +84,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="167" formatCode="mmm/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -126,6 +132,12 @@
       <name val="Times New Roman"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -328,7 +340,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -336,7 +348,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -421,7 +433,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -437,10 +449,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -489,7 +497,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -575,7 +583,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -673,68 +681,72 @@
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="G6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="F7" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="22"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="28"/>
+        <v>16</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="36.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="28"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="28"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,33 +754,33 @@
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="A15" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>